<commit_message>
WIP commit: Working on FoodItem testing suite
</commit_message>
<xml_diff>
--- a/docs/EasyFPUTesting.xlsx
+++ b/docs/EasyFPUTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrich/Repositories/iOS-EasyFPU/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF4A16B-DBF2-2D43-B7A8-8840B24DA1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746D932F-72DE-7B4F-9382-CD83A2E4F3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="920" windowWidth="28240" windowHeight="17240" xr2:uid="{B16DE3F7-D17F-9E4A-AD07-F0528E382159}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -90,6 +90,63 @@
   </si>
   <si>
     <t>Delete all FoodItems and ComposedFoodItems, cascading deletion of TypicalAmounts (with FoodItems) and Ingredients (with ComposedFoodItems) - all named tables empty</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>FoodItem.create(from composedFoodItem: ComposedFoodItemViewModel)</t>
+  </si>
+  <si>
+    <t>FoodItem with identical ID as ComposedFoodItemVM in DB</t>
+  </si>
+  <si>
+    <t>Return new FoodItem, FoodItem count in DB = 1, TypicalAmount count in DB = 8</t>
+  </si>
+  <si>
+    <t>Return existing FoodItem, FoodItem count in DB = 1, TypicalAmount count in DB = 8</t>
+  </si>
+  <si>
+    <t>FoodItem.update(_ cdFoodItem: FoodItem, with foodItemVM: FoodItemViewModel, _ typicalAmountsToBeDeleted: [TypicalAmountViewModel])</t>
+  </si>
+  <si>
+    <t>No related Ingredient exists</t>
+  </si>
+  <si>
+    <t>Updated FoodItem has same values as modified FoodItemViewModel</t>
+  </si>
+  <si>
+    <t>A related Ingredient exists and also a ComposedFoodItem the Ingredient relates to</t>
+  </si>
+  <si>
+    <t>Updated FoodItem and Ingredient have same values as modified FoodItemViewModel</t>
+  </si>
+  <si>
+    <t>No related FoodItem exists, no FoodItem in DB</t>
+  </si>
+  <si>
+    <t>Test suite</t>
+  </si>
+  <si>
+    <t>CoreDataTests.FoodItemBehavior</t>
+  </si>
+  <si>
+    <t>CoreDataTests.CombinedFunctionality</t>
+  </si>
+  <si>
+    <t>typicalAmountsToBeDeleted = []</t>
+  </si>
+  <si>
+    <t>typicalAmountsToBeDeleted = [a few typicalAmountVMs]</t>
+  </si>
+  <si>
+    <t>Updated FoodItem has same values as modified FoodItemViewModel, the specified TypicalAmounts are deleted</t>
   </si>
 </sst>
 </file>
@@ -137,9 +194,9 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -151,7 +208,13 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -170,14 +233,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B7BD6A0-AD6D-4242-9982-5DA5A94EC092}" name="Tabelle1" displayName="Tabelle1" ref="A1:E14" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E14" xr:uid="{4B7BD6A0-AD6D-4242-9982-5DA5A94EC092}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{01AF1201-33A2-D14F-BFAC-31BE6E750A68}" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{48C18B24-42CE-8F44-8F36-785FD430DA30}" name="Main tested function" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B7BD6A0-AD6D-4242-9982-5DA5A94EC092}" name="Tabelle1" displayName="Tabelle1" ref="A1:G18" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:G18" xr:uid="{4B7BD6A0-AD6D-4242-9982-5DA5A94EC092}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{01AF1201-33A2-D14F-BFAC-31BE6E750A68}" name="ID" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{3FC64CE9-059D-6641-AD94-3594B07DCA04}" name="Test suite" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{48C18B24-42CE-8F44-8F36-785FD430DA30}" name="Main tested function" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{3F39B9F4-2DB3-F146-8294-8671D1359054}" name="Test parameters" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{3C2F157B-7697-C348-9245-946AB4D67875}" name="Prerequisites" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{72BE5D49-E6DB-524A-AD76-569FF8F40D8E}" name="Expected result" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{3C2F157B-7697-C348-9245-946AB4D67875}" name="Prerequisites" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{72BE5D49-E6DB-524A-AD76-569FF8F40D8E}" name="Expected result" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{2C3433CB-EC87-B34E-A9BA-4CAE10AAA493}" name="Implemented" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -500,192 +565,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4AD339-B7F2-6946-83F8-46C76F46AB0E}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C20:C21"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="66.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="43.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" customWidth="1"/>
+    <col min="4" max="6" width="43.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="E13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Finished Unit Tests for FoodItem
</commit_message>
<xml_diff>
--- a/docs/EasyFPUTesting.xlsx
+++ b/docs/EasyFPUTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrich/Repositories/iOS-EasyFPU/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746D932F-72DE-7B4F-9382-CD83A2E4F3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4942310-A22D-F848-8DE0-CB8F53D233EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="920" windowWidth="28240" windowHeight="17240" xr2:uid="{B16DE3F7-D17F-9E4A-AD07-F0528E382159}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -147,6 +147,24 @@
   </si>
   <si>
     <t>Updated FoodItem has same values as modified FoodItemViewModel, the specified TypicalAmounts are deleted</t>
+  </si>
+  <si>
+    <t>FoodItem.duplicate(_ existingFoodItem: FoodItem)</t>
+  </si>
+  <si>
+    <t>2 FoodItems in DB, different names, different IDs, rest the same, same typical amounts</t>
+  </si>
+  <si>
+    <t>FoodItem.add(_ typicalAmount: TypicalAmount, to foodItem: FoodItem)</t>
+  </si>
+  <si>
+    <t>TypicalAmount added to DB and linked to FoodItem</t>
+  </si>
+  <si>
+    <t>FoodItem.setCategory(_ foodItem: FoodItem?, to category: String)</t>
+  </si>
+  <si>
+    <t>Changed category</t>
   </si>
 </sst>
 </file>
@@ -196,16 +214,7 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -215,6 +224,15 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -233,16 +251,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B7BD6A0-AD6D-4242-9982-5DA5A94EC092}" name="Tabelle1" displayName="Tabelle1" ref="A1:G18" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A1:G18" xr:uid="{4B7BD6A0-AD6D-4242-9982-5DA5A94EC092}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B7BD6A0-AD6D-4242-9982-5DA5A94EC092}" name="Tabelle1" displayName="Tabelle1" ref="A1:G25" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:G25" xr:uid="{4B7BD6A0-AD6D-4242-9982-5DA5A94EC092}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{01AF1201-33A2-D14F-BFAC-31BE6E750A68}" name="ID" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{3FC64CE9-059D-6641-AD94-3594B07DCA04}" name="Test suite" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{48C18B24-42CE-8F44-8F36-785FD430DA30}" name="Main tested function" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{3F39B9F4-2DB3-F146-8294-8671D1359054}" name="Test parameters" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{3C2F157B-7697-C348-9245-946AB4D67875}" name="Prerequisites" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{72BE5D49-E6DB-524A-AD76-569FF8F40D8E}" name="Expected result" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{2C3433CB-EC87-B34E-A9BA-4CAE10AAA493}" name="Implemented" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{01AF1201-33A2-D14F-BFAC-31BE6E750A68}" name="ID" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{3FC64CE9-059D-6641-AD94-3594B07DCA04}" name="Test suite" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{48C18B24-42CE-8F44-8F36-785FD430DA30}" name="Main tested function" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{3F39B9F4-2DB3-F146-8294-8671D1359054}" name="Test parameters" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{3C2F157B-7697-C348-9245-946AB4D67875}" name="Prerequisites" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{72BE5D49-E6DB-524A-AD76-569FF8F40D8E}" name="Expected result" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{2C3433CB-EC87-B34E-A9BA-4CAE10AAA493}" name="Implemented" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -565,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4AD339-B7F2-6946-83F8-46C76F46AB0E}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -778,50 +796,72 @@
       <c r="F9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -860,20 +900,91 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP commit: Unit testing ComposedFoodItem Core Data operations
</commit_message>
<xml_diff>
--- a/docs/EasyFPUTesting.xlsx
+++ b/docs/EasyFPUTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrich/Repositories/iOS-EasyFPU/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4942310-A22D-F848-8DE0-CB8F53D233EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35803AD5-356D-4F4F-BC9C-03820F72CE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="920" windowWidth="28240" windowHeight="17240" xr2:uid="{B16DE3F7-D17F-9E4A-AD07-F0528E382159}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -165,6 +165,21 @@
   </si>
   <si>
     <t>Changed category</t>
+  </si>
+  <si>
+    <t>CoreDataTests.ComposedFoodItemBehavior</t>
+  </si>
+  <si>
+    <t>ComposedFoodItem.create(from composedFoodItemVM: ComposedFoodItemViewModel, _ isImport: Bool)</t>
+  </si>
+  <si>
+    <t>Empty DB</t>
+  </si>
+  <si>
+    <t>isImport = true</t>
+  </si>
+  <si>
+    <t>ComposedFoodItem, its related FoodItem, all related Ingredients and their related FoodItems are created</t>
   </si>
 </sst>
 </file>
@@ -586,14 +601,15 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67.6640625" customWidth="1"/>
-    <col min="4" max="6" width="43.1640625" customWidth="1"/>
+    <col min="4" max="5" width="43.1640625" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -853,16 +869,32 @@
       <c r="F12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>

</xml_diff>

<commit_message>
WIP commit: Continue unit testing ComposedFoodItem
</commit_message>
<xml_diff>
--- a/docs/EasyFPUTesting.xlsx
+++ b/docs/EasyFPUTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrich/Repositories/iOS-EasyFPU/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35803AD5-356D-4F4F-BC9C-03820F72CE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ECB113-C944-D148-8415-60E78D73D729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="920" windowWidth="28240" windowHeight="17240" xr2:uid="{B16DE3F7-D17F-9E4A-AD07-F0528E382159}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>ComposedFoodItem, its related FoodItem, all related Ingredients and their related FoodItems are created</t>
+  </si>
+  <si>
+    <t>isImport = false</t>
+  </si>
+  <si>
+    <t>ComposedFoodItemVM with ingredients, which already exist as FoodItems in the DB</t>
+  </si>
+  <si>
+    <t>ComposedFoodItem.update(_ composedFoodItemVM: ComposedFoodItemViewModel)</t>
+  </si>
+  <si>
+    <t>A fully available ComposedFoodItem with related FoodItem, Ingredients and their FoodItems</t>
   </si>
 </sst>
 </file>
@@ -600,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4AD339-B7F2-6946-83F8-46C76F46AB0E}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,21 +908,43 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>

</xml_diff>